<commit_message>
commit backend ver 1
</commit_message>
<xml_diff>
--- a/backend/data/TestData.xlsx
+++ b/backend/data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohanganadal/Data Company/Avisk GHG Emisstion Calculator/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8976C19E-9FA4-3C49-89AB-D4F8C9A997C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C3DC8A-33ED-B14A-9F0B-2D458864E89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20300" xr2:uid="{C8F1BE37-6A66-8343-9BA6-C4D31E4D0BE5}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <definedName name="Ref_DD_Region">'[1]Reference - Lookup and Unit'!$A$36:$A$38</definedName>
     <definedName name="Ref_DD_TransportMode">'[1]Reference - Lookup and Unit'!$A$43:$A$46</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t>Source/Description</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Total Weight of Freight (tonne)</t>
-  </si>
-  <si>
-    <t># of Passengers</t>
   </si>
   <si>
     <t>Units of Measurement (Tonne Miles)</t>
@@ -122,7 +119,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -193,10 +190,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -205,11 +201,7 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -218,42 +210,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Stationary_combustion_tool_GL1" xfId="1" xr:uid="{40021526-D014-DC43-956E-E633D0BCAAAE}"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="gray125"/>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill patternType="gray125"/>
@@ -688,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD8B373-77B7-024F-BBE6-48409D4BB287}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="J2" sqref="J2:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -704,14 +661,13 @@
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -748,192 +704,176 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1000</v>
+      </c>
+      <c r="H2" s="4">
+        <v>381.6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1000</v>
+      </c>
+      <c r="H3" s="4">
+        <v>381.6</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G4" s="3">
+        <v>1000</v>
+      </c>
+      <c r="H4" s="4">
+        <v>381.6</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="4">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="3">
         <v>1000</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H5" s="4">
         <v>381.6</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="3" t="s">
+      <c r="I5" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G6" s="3">
+        <v>1000</v>
+      </c>
+      <c r="H6" s="4">
+        <v>381.6</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="G3" s="4">
-        <v>1000</v>
-      </c>
-      <c r="H3" s="5">
-        <v>381.6</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1000</v>
-      </c>
-      <c r="H4" s="5">
-        <v>381.6</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1000</v>
-      </c>
-      <c r="H5" s="5">
-        <v>381.6</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="4">
-        <v>1000</v>
-      </c>
-      <c r="H6" s="5">
-        <v>381.6</v>
-      </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="F2:F6">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
       <formula>$G2="Custom Fuel"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
       <formula>AND($G2="Fuel Use",$D2="Other")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6 J2:J6">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="G2:G6 I2:I6">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
       <formula>OR($G2="Custom Fuel",$G2="Fuel Use")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H6">
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
-      <formula>$CR2="Custom Fuel"</formula>
+    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
+      <formula>$CQ2="Custom Fuel"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
-      <formula>AND($CR2&lt;&gt;"Weight Distance (e.g. Freight Transport)",$G2&lt;&gt;0)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I6">
-    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
-      <formula>AND($CR2&lt;&gt;"Passenger Distance (e.g. Public Transport)",$CR2&lt;&gt;0)</formula>
+    <cfRule type="expression" dxfId="0" priority="8" stopIfTrue="1">
+      <formula>AND($CQ2&lt;&gt;"Weight Distance (e.g. Freight Transport)",$G2&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F6" xr:uid="{E8B16885-8630-2C4F-B297-3A8E50459D99}">
-      <formula1>INDIRECT(IF($G2="Custom Vehicle","Settings_Custom_Vehicle",IF($AY2=TRUE,$AT2,"Ref_DD_NA")))</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6" xr:uid="{4038273B-9C48-D646-9DC8-6B1B7C079E3B}">
       <formula1>Ref_DD_TransportMode</formula1>
     </dataValidation>
@@ -943,11 +883,14 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:E6" xr:uid="{FFC65A44-55D3-324C-8DB3-0E06A25A9950}">
       <formula1>INDIRECT(IF(AND($D2&lt;&gt;"US",$F2="Scope 1"),"Ref_DD_NonUK",IF($F2="Scope 1","Ref_DD_ActivityData_Rail","Ref_DD_Scope3")))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J6" xr:uid="{72A5476D-6E9D-6F4C-980F-B1B2E9A7D8EB}">
-      <formula1>INDIRECT($CP2)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I6" xr:uid="{72A5476D-6E9D-6F4C-980F-B1B2E9A7D8EB}">
+      <formula1>INDIRECT($CO2)</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:I6" xr:uid="{26C3AA86-B09A-754C-90F6-3CE00EA09D0C}">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H6" xr:uid="{26C3AA86-B09A-754C-90F6-3CE00EA09D0C}">
       <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F6" xr:uid="{E8B16885-8630-2C4F-B297-3A8E50459D99}">
+      <formula1>INDIRECT(IF($G2="Custom Vehicle","Settings_Custom_Vehicle",IF($AX2=TRUE,$AS2,"Ref_DD_NA")))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>